<commit_message>
inserindo lógica para inc matriz
</commit_message>
<xml_diff>
--- a/Incidentes_Formatados_Final.xlsx
+++ b/Incidentes_Formatados_Final.xlsx
@@ -127,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -203,8 +203,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="6" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="6" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -708,94 +723,95 @@
     <row r="2" ht="75" customHeight="1">
       <c r="A2" s="26" t="inlineStr">
         <is>
-          <t>Loja 181</t>
+          <t>MATRIZ TI - Cuiabá</t>
         </is>
       </c>
       <c r="B2" s="26" t="inlineStr">
         <is>
-          <t>R10 - Mizael</t>
-        </is>
-      </c>
-      <c r="C2" s="26" t="inlineStr">
-        <is>
-          <t>09:00</t>
-        </is>
-      </c>
-      <c r="D2" s="26" t="inlineStr">
+          <t>ADM</t>
+        </is>
+      </c>
+      <c r="C2" s="27" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="D2" s="27" t="inlineStr">
         <is>
           <t>22:00</t>
         </is>
       </c>
       <c r="E2" s="26" t="inlineStr">
         <is>
-          <t>FIREWALL TRAVADO</t>
+          <t>LINK INOPERANTE</t>
         </is>
       </c>
       <c r="F2" s="26" t="inlineStr">
         <is>
-          <t>FIREWALL</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="G2" s="26" t="inlineStr">
         <is>
-          <t>PARCIAL</t>
+          <t>INOPERANTE</t>
         </is>
       </c>
       <c r="H2" s="26" t="inlineStr">
         <is>
-          <t>NENHUM</t>
-        </is>
-      </c>
-      <c r="I2" s="26" t="inlineStr">
-        <is>
-          <t>26/06/2025</t>
-        </is>
-      </c>
-      <c r="J2" s="26" t="inlineStr">
-        <is>
-          <t>25/06/2025 15:39</t>
-        </is>
-      </c>
-      <c r="K2" s="26" t="inlineStr">
-        <is>
-          <t>25/06/2025 16:41</t>
-        </is>
-      </c>
-      <c r="L2" s="26" t="inlineStr">
-        <is>
-          <t>01:02</t>
-        </is>
-      </c>
-      <c r="M2" s="26" t="inlineStr">
-        <is>
-          <t>11:58</t>
+          <t>OI DEDICADO</t>
+        </is>
+      </c>
+      <c r="I2" s="28" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J2" s="29" t="inlineStr">
+        <is>
+          <t>29/06/2025 14:18</t>
+        </is>
+      </c>
+      <c r="K2" s="29" t="inlineStr">
+        <is>
+          <t>29/06/2025 16:50</t>
+        </is>
+      </c>
+      <c r="L2" s="30" t="inlineStr">
+        <is>
+          <t>02:32</t>
+        </is>
+      </c>
+      <c r="M2" s="27" t="inlineStr">
+        <is>
+          <t>09:28</t>
         </is>
       </c>
       <c r="N2" s="26" t="inlineStr">
         <is>
-          <t>Foi identificado que o Firewall da loja travou, causando indisponibilidade na conexão com a internet, durante o incidente a loja ficou VENDENDO OFFLINE, resolvido com a reinicialização dos FWs em Loja, conexão normalizada. Aberto chamado com o time do SOC para analisar os equipamentos e verificar se está tudo certo com os firewalls da loja.</t>
-        </is>
-      </c>
+          <t>Chamado Callcenter Matriz, foi identificado indisponibilidade nas ligações receptivas, callcenter conseguindo efetuar ligações mas sem receber, reportado pela operadora que o problema estava relacionado a uma falha massiva nos canais de voz, callcenter normalizado sem mais informações sobre a causa do problema. Validado com o time de Suporte</t>
+        </is>
+      </c>
+      <c r="O2" s="26" t="n"/>
     </row>
     <row r="3" ht="75" customHeight="1">
       <c r="A3" s="26" t="inlineStr">
         <is>
-          <t>Loja 161</t>
+          <t>Loja 102</t>
         </is>
       </c>
       <c r="B3" s="26" t="inlineStr">
         <is>
-          <t>R05 - Diely</t>
-        </is>
-      </c>
-      <c r="C3" s="26" t="inlineStr">
-        <is>
-          <t>07:00</t>
-        </is>
-      </c>
-      <c r="D3" s="26" t="inlineStr">
-        <is>
-          <t>19:00</t>
+          <t>R03 - Hanna</t>
+        </is>
+      </c>
+      <c r="C3" s="31" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D3" s="31" t="inlineStr">
+        <is>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E3" s="26" t="inlineStr">
@@ -815,74 +831,75 @@
       </c>
       <c r="H3" s="26" t="inlineStr">
         <is>
-          <t>OI DEDICADO</t>
-        </is>
-      </c>
-      <c r="I3" s="26" t="inlineStr">
-        <is>
-          <t>26/06/2025</t>
-        </is>
-      </c>
-      <c r="J3" s="26" t="inlineStr">
-        <is>
-          <t>25/06/2025 07:00</t>
-        </is>
-      </c>
-      <c r="K3" s="26" t="inlineStr">
-        <is>
-          <t>25/06/2025 09:00</t>
-        </is>
-      </c>
-      <c r="L3" s="26" t="inlineStr">
-        <is>
-          <t>02:00</t>
-        </is>
-      </c>
-      <c r="M3" s="26" t="inlineStr">
-        <is>
-          <t>10:00</t>
+          <t>NENHUM</t>
+        </is>
+      </c>
+      <c r="I3" s="28" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J3" s="32" t="inlineStr">
+        <is>
+          <t>29/06/2025 06:00</t>
+        </is>
+      </c>
+      <c r="K3" s="32" t="inlineStr">
+        <is>
+          <t>29/06/2025 09:02</t>
+        </is>
+      </c>
+      <c r="L3" s="30" t="inlineStr">
+        <is>
+          <t>01:02</t>
+        </is>
+      </c>
+      <c r="M3" s="27" t="inlineStr">
+        <is>
+          <t>11:58</t>
         </is>
       </c>
       <c r="N3" s="26" t="inlineStr">
         <is>
-          <t>Identificado problema referente ao quadro de energia, um curto em um fusível do painel de energia, Nobreak sustentou a loja até o fim da autonomia, Gerente acompanhou o time de manutenção na correção do quadro de energia, energia normalizada, VMs e APIs religadas, Loja operando novamente.</t>
-        </is>
-      </c>
+          <t>Foi identificado queda de energia durante a madrugada, energia normalizada, Servidor, VMs e APIs Up novamente, Loja normalizada, validado por Jessica.</t>
+        </is>
+      </c>
+      <c r="O3" s="26" t="n"/>
     </row>
     <row r="4" ht="75" customHeight="1">
       <c r="A4" s="26" t="inlineStr">
         <is>
-          <t>Loja 47</t>
+          <t>Loja 129</t>
         </is>
       </c>
       <c r="B4" s="26" t="inlineStr">
         <is>
-          <t>R08 - Edimar</t>
-        </is>
-      </c>
-      <c r="C4" s="26" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="D4" s="26" t="inlineStr">
+          <t>R02 - Jonatas</t>
+        </is>
+      </c>
+      <c r="C4" s="31" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="D4" s="31" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
       <c r="E4" s="26" t="inlineStr">
         <is>
-          <t>SERVIDOR DESLIGADO</t>
+          <t>LINK INTERMITENTE</t>
         </is>
       </c>
       <c r="F4" s="26" t="inlineStr">
         <is>
-          <t>SERVIÇO</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="G4" s="26" t="inlineStr">
         <is>
-          <t>INOPERANTE</t>
+          <t>PARCIAL</t>
         </is>
       </c>
       <c r="H4" s="26" t="inlineStr">
@@ -890,66 +907,67 @@
           <t>NENHUM</t>
         </is>
       </c>
-      <c r="I4" s="26" t="inlineStr">
-        <is>
-          <t>26/06/2025</t>
-        </is>
-      </c>
-      <c r="J4" s="26" t="inlineStr">
-        <is>
-          <t>24/06/2025 17:36</t>
-        </is>
-      </c>
-      <c r="K4" s="26" t="inlineStr">
-        <is>
-          <t>24/06/2025 19:00</t>
-        </is>
-      </c>
-      <c r="L4" s="26" t="inlineStr">
-        <is>
-          <t>01:24</t>
-        </is>
-      </c>
-      <c r="M4" s="26" t="inlineStr">
-        <is>
-          <t>09:36</t>
+      <c r="I4" s="28" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J4" s="32" t="inlineStr">
+        <is>
+          <t>28/06/2025 10:30</t>
+        </is>
+      </c>
+      <c r="K4" s="32" t="inlineStr">
+        <is>
+          <t>28/06/2025 18:00</t>
+        </is>
+      </c>
+      <c r="L4" s="30" t="inlineStr">
+        <is>
+          <t>07:30</t>
+        </is>
+      </c>
+      <c r="M4" s="27" t="inlineStr">
+        <is>
+          <t>04:30</t>
         </is>
       </c>
       <c r="N4" s="26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Loja desligou os equipamentos do rack de forma preventiva devido a chuva forte que alagou a sala da TI. Ficou no aguardo um retorno da loja para tratativa.  </t>
-        </is>
-      </c>
+          <t>Foi identificado que ambos os links da loja ficaram intermitentes, causando indisponibilidade no VAR, feito a virada manual da loja pra offline pelo time de Sistemas em WR, como um paliativo para seguir vendendo até a normalização dos links, loja seguiu na modalidade de venda offline até o encerramento do expediente, Loja validada no dia seguinte (Domingo) na abertura.</t>
+        </is>
+      </c>
+      <c r="O4" s="26" t="n"/>
     </row>
     <row r="5" ht="75" customHeight="1">
       <c r="A5" s="26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Loja 119 </t>
+          <t>Loja 62</t>
         </is>
       </c>
       <c r="B5" s="26" t="inlineStr">
         <is>
-          <t>R07 - Willian Beycon</t>
-        </is>
-      </c>
-      <c r="C5" s="26" t="inlineStr">
-        <is>
-          <t>07:00</t>
-        </is>
-      </c>
-      <c r="D5" s="26" t="inlineStr">
+          <t>R05 - Diely</t>
+        </is>
+      </c>
+      <c r="C5" s="31" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D5" s="31" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
       <c r="E5" s="26" t="inlineStr">
         <is>
-          <t>LINK INOPERANTE</t>
+          <t>FALTA DE ENERGIA</t>
         </is>
       </c>
       <c r="F5" s="26" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>ENERGIA</t>
         </is>
       </c>
       <c r="G5" s="26" t="inlineStr">
@@ -959,137 +977,1356 @@
       </c>
       <c r="H5" s="26" t="inlineStr">
         <is>
-          <t>NENHUM</t>
-        </is>
-      </c>
-      <c r="I5" s="26" t="inlineStr">
-        <is>
-          <t>26/06/2025</t>
-        </is>
-      </c>
-      <c r="J5" s="26" t="inlineStr">
-        <is>
-          <t>24/06/2025 17:35</t>
-        </is>
-      </c>
-      <c r="K5" s="26" t="inlineStr">
-        <is>
-          <t>24/06/2025 17:50</t>
-        </is>
-      </c>
-      <c r="L5" s="26" t="inlineStr">
-        <is>
-          <t>00:15</t>
-        </is>
-      </c>
-      <c r="M5" s="26" t="inlineStr">
-        <is>
-          <t>11:45</t>
+          <t>OI DEDICADO</t>
+        </is>
+      </c>
+      <c r="I5" s="28" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J5" s="32" t="inlineStr">
+        <is>
+          <t>28/06/2025 08:11</t>
+        </is>
+      </c>
+      <c r="K5" s="32" t="inlineStr">
+        <is>
+          <t>28/06/2025 10:40</t>
+        </is>
+      </c>
+      <c r="L5" s="30" t="inlineStr">
+        <is>
+          <t>02:29</t>
+        </is>
+      </c>
+      <c r="M5" s="27" t="inlineStr">
+        <is>
+          <t>08:31</t>
         </is>
       </c>
       <c r="N5" s="26" t="inlineStr">
         <is>
-          <t>Loja se encontrava sem sistema Var para operações devido a ambos os links terem ficado down. Confirmado com o suporte que a loja estava vendendo offline até a normalização do link. Aberto chamado com a operadora para verificação, o link secundário ficou up e estável então foi solicitado ao suporte acompanhar a loja em um teste de venda e validar a VENDA ONLINE, que foi validado pela Larissa. Sem retorno da operadora quanto a solução. Protocolo Link principal: 91855659895 | Protocolo Link Secundário: 91855660874.</t>
-        </is>
-      </c>
+          <t>Foi identificado queda de energia na Loja, loja operou com caixas reduzidos e sendo sustentada pelo Nobreak nesse período, equipe de manutenção se deslocou pra loja para levar um gerador, porem a energia normalizou e não foi necessário, Loja normalizada.</t>
+        </is>
+      </c>
+      <c r="O5" s="26" t="n"/>
     </row>
     <row r="6" ht="75" customHeight="1">
       <c r="A6" s="26" t="inlineStr">
         <is>
+          <t>LOJA 185</t>
+        </is>
+      </c>
+      <c r="B6" s="26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Selecionar </t>
+        </is>
+      </c>
+      <c r="C6" s="31" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D6" s="31" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="E6" s="26" t="inlineStr">
+        <is>
+          <t>LINK INOPERANTE</t>
+        </is>
+      </c>
+      <c r="F6" s="26" t="inlineStr">
+        <is>
+          <t>FIREWALL</t>
+        </is>
+      </c>
+      <c r="G6" s="26" t="inlineStr">
+        <is>
+          <t>INOPERANTE</t>
+        </is>
+      </c>
+      <c r="H6" s="26" t="inlineStr">
+        <is>
+          <t>NENHUM</t>
+        </is>
+      </c>
+      <c r="I6" s="28" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J6" s="32" t="inlineStr">
+        <is>
+          <t>27/06/2025 15:20</t>
+        </is>
+      </c>
+      <c r="K6" s="32" t="inlineStr">
+        <is>
+          <t>27/06/2025 16:35</t>
+        </is>
+      </c>
+      <c r="L6" s="30" t="inlineStr">
+        <is>
+          <t>01:15</t>
+        </is>
+      </c>
+      <c r="M6" s="27" t="inlineStr">
+        <is>
+          <t>08:45</t>
+        </is>
+      </c>
+      <c r="N6" s="26" t="inlineStr">
+        <is>
+          <t>Loja parou de responder para o google e o dns do google, por conta disso a Loja foi virada para o OFFLINE devido ao link secundário ter ficado down e ao travamento/falha de sincronização do firewall e o link principal estava UP porém com perda de pacote. O suporte solicitou ao time de sistemas a mudança dos endereços para o dns e a url da matriz. Equipe de redes  em conjunto com a gerente reiniciou o Firewall para sincronização. Após atuação da equipe foi realizado teste de venda acompanhado pelo suporte e validado pela Mayane.</t>
+        </is>
+      </c>
+      <c r="O6" s="26" t="n"/>
+    </row>
+    <row r="7" ht="75" customHeight="1">
+      <c r="A7" s="26" t="inlineStr">
+        <is>
+          <t>Loja 52</t>
+        </is>
+      </c>
+      <c r="B7" s="26" t="inlineStr">
+        <is>
+          <t>R09 - Edimar</t>
+        </is>
+      </c>
+      <c r="C7" s="31" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D7" s="31" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="E7" s="26" t="inlineStr">
+        <is>
+          <t>FALTA DE ENERGIA</t>
+        </is>
+      </c>
+      <c r="F7" s="26" t="inlineStr">
+        <is>
+          <t>ENERGIA</t>
+        </is>
+      </c>
+      <c r="G7" s="26" t="inlineStr">
+        <is>
+          <t>INOPERANTE</t>
+        </is>
+      </c>
+      <c r="H7" s="26" t="inlineStr">
+        <is>
+          <t>NENHUM</t>
+        </is>
+      </c>
+      <c r="I7" s="28" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J7" s="32" t="inlineStr">
+        <is>
+          <t>27/06/2025 07:00</t>
+        </is>
+      </c>
+      <c r="K7" s="32" t="inlineStr">
+        <is>
+          <t>27/06/2025 10:10</t>
+        </is>
+      </c>
+      <c r="L7" s="30" t="inlineStr">
+        <is>
+          <t>02:10</t>
+        </is>
+      </c>
+      <c r="M7" s="27" t="inlineStr">
+        <is>
+          <t>09:50</t>
+        </is>
+      </c>
+      <c r="N7" s="26" t="inlineStr">
+        <is>
+          <t>Equipamentos sem resposta, identificado a queda de energia na loja durante a madrugada. O firewall precisou ser reiniciado para ocorrer a sincronização com os equipamentos. Solicitado ao suporte realizar teste de venda. Validado com Cátia.</t>
+        </is>
+      </c>
+      <c r="O7" s="26" t="n"/>
+    </row>
+    <row r="8" ht="75" customHeight="1">
+      <c r="A8" s="26" t="inlineStr">
+        <is>
+          <t>Loja 102</t>
+        </is>
+      </c>
+      <c r="B8" s="26" t="inlineStr">
+        <is>
+          <t>R03 - Hanna</t>
+        </is>
+      </c>
+      <c r="C8" s="31" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D8" s="31" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="E8" s="26" t="inlineStr">
+        <is>
+          <t>SERVIDOR DESLIGADO</t>
+        </is>
+      </c>
+      <c r="F8" s="26" t="inlineStr">
+        <is>
+          <t>ENERGIA</t>
+        </is>
+      </c>
+      <c r="G8" s="26" t="inlineStr">
+        <is>
+          <t>INOPERANTE</t>
+        </is>
+      </c>
+      <c r="H8" s="26" t="inlineStr">
+        <is>
+          <t>NENHUM</t>
+        </is>
+      </c>
+      <c r="I8" s="28" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J8" s="32" t="inlineStr">
+        <is>
+          <t>27/06/2025 07:00</t>
+        </is>
+      </c>
+      <c r="K8" s="32" t="inlineStr">
+        <is>
+          <t>27/06/2025 08:21</t>
+        </is>
+      </c>
+      <c r="L8" s="30" t="inlineStr">
+        <is>
+          <t>00:21</t>
+        </is>
+      </c>
+      <c r="M8" s="27" t="inlineStr">
+        <is>
+          <t>12:39</t>
+        </is>
+      </c>
+      <c r="N8" s="26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Todos os equipamentos da loja sem resposta. Colaboradora informou que o disjuntor estava para baixo, desligado. Assim que o disjuntor foi religado os equipamentos ficaram todos ups novamente. Solicitado ao suporte acompanhar a loja em um teste de venda que foi validado pela Jessica.
+</t>
+        </is>
+      </c>
+      <c r="O8" s="26" t="n"/>
+    </row>
+    <row r="9" ht="75" customHeight="1">
+      <c r="A9" s="26" t="inlineStr">
+        <is>
+          <t>Loja 129</t>
+        </is>
+      </c>
+      <c r="B9" s="26" t="inlineStr">
+        <is>
+          <t>R02 - Jonatas</t>
+        </is>
+      </c>
+      <c r="C9" s="31" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="D9" s="31" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E9" s="26" t="inlineStr">
+        <is>
+          <t>SWITCH TRAVADO</t>
+        </is>
+      </c>
+      <c r="F9" s="26" t="inlineStr">
+        <is>
+          <t>SWITCH</t>
+        </is>
+      </c>
+      <c r="G9" s="26" t="inlineStr">
+        <is>
+          <t>INOPERANTE</t>
+        </is>
+      </c>
+      <c r="H9" s="26" t="inlineStr">
+        <is>
+          <t>OI DEDICADO</t>
+        </is>
+      </c>
+      <c r="I9" s="28" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J9" s="32" t="inlineStr">
+        <is>
+          <t>27/06/2025 06:00</t>
+        </is>
+      </c>
+      <c r="K9" s="32" t="inlineStr">
+        <is>
+          <t>27/06/2025 09:00</t>
+        </is>
+      </c>
+      <c r="L9" s="30" t="inlineStr">
+        <is>
+          <t>02:00</t>
+        </is>
+      </c>
+      <c r="M9" s="27" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="N9" s="26" t="inlineStr">
+        <is>
+          <t>Links e fw UP, porém demais equipamentos sem resposta devido aos switches da loja terem travado. Os equipamentos voltaram a funcionar assim que a equipe de redes reiniciou o firewall e os switches. Suporte acompanhou a loja em um teste de venda que foi validado em WR.</t>
+        </is>
+      </c>
+      <c r="O9" s="26" t="n"/>
+    </row>
+    <row r="10" ht="75" customHeight="1">
+      <c r="A10" s="26" t="inlineStr">
+        <is>
+          <t>MATRIZ TI - Cuiabá</t>
+        </is>
+      </c>
+      <c r="B10" s="26" t="inlineStr">
+        <is>
+          <t>R01 - Enivaldo Mariano</t>
+        </is>
+      </c>
+      <c r="C10" s="31" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="D10" s="31" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="E10" s="26" t="inlineStr">
+        <is>
+          <t>LINK INOPERANTE</t>
+        </is>
+      </c>
+      <c r="F10" s="26" t="inlineStr">
+        <is>
+          <t>SERVIÇO</t>
+        </is>
+      </c>
+      <c r="G10" s="26" t="inlineStr">
+        <is>
+          <t>PARCIAL</t>
+        </is>
+      </c>
+      <c r="H10" s="26" t="inlineStr">
+        <is>
+          <t>OI DEDICADO</t>
+        </is>
+      </c>
+      <c r="I10" s="28" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J10" s="32" t="inlineStr">
+        <is>
+          <t>26/06/2025 15:18</t>
+        </is>
+      </c>
+      <c r="K10" s="32" t="inlineStr">
+        <is>
+          <t>26/06/2025 16:46</t>
+        </is>
+      </c>
+      <c r="L10" s="30" t="inlineStr">
+        <is>
+          <t>01:28</t>
+        </is>
+      </c>
+      <c r="M10" s="27" t="inlineStr">
+        <is>
+          <t>08:32</t>
+        </is>
+      </c>
+      <c r="N10" s="26" t="inlineStr">
+        <is>
+          <t>Foi informado que o call center não estava realizando, nem recebendo ligações externas. Em uma call com as equipes da Oi e da Next foram feitos diversos testes em conjunto porém a causa não foi identificada. Central foi normalizada, porém ficou pendente de análise no equipamento KHOMP (NextIP) verificar a origem da falha. Validação realizada junto ao suporte referente as ligações entrantes e saíntes.</t>
+        </is>
+      </c>
+      <c r="O10" s="26" t="n"/>
+    </row>
+    <row r="11" ht="75" customHeight="1">
+      <c r="A11" s="26" t="inlineStr">
+        <is>
+          <t>Loja 181</t>
+        </is>
+      </c>
+      <c r="B11" s="26" t="inlineStr">
+        <is>
+          <t>R10 - Mizael</t>
+        </is>
+      </c>
+      <c r="C11" s="31" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D11" s="31" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="E11" s="26" t="inlineStr">
+        <is>
+          <t>FIREWALL TRAVADO</t>
+        </is>
+      </c>
+      <c r="F11" s="26" t="inlineStr">
+        <is>
+          <t>FIREWALL</t>
+        </is>
+      </c>
+      <c r="G11" s="26" t="inlineStr">
+        <is>
+          <t>PARCIAL</t>
+        </is>
+      </c>
+      <c r="H11" s="26" t="inlineStr">
+        <is>
+          <t>NENHUM</t>
+        </is>
+      </c>
+      <c r="I11" s="28" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J11" s="32" t="inlineStr">
+        <is>
+          <t>25/06/2025 15:39</t>
+        </is>
+      </c>
+      <c r="K11" s="32" t="inlineStr">
+        <is>
+          <t>25/06/2025 16:41</t>
+        </is>
+      </c>
+      <c r="L11" s="30" t="inlineStr">
+        <is>
+          <t>01:02</t>
+        </is>
+      </c>
+      <c r="M11" s="27" t="inlineStr">
+        <is>
+          <t>11:58</t>
+        </is>
+      </c>
+      <c r="N11" s="26" t="inlineStr">
+        <is>
+          <t>Foi identificado que o Firewall da loja travou, causando indisponibilidade na conexão com a internet, durante o incidente a loja ficou VENDENDO OFFLINE, resolvido com a reinicialização dos FWs em Loja, conexão normalizada. Aberto chamado com o time do SOC para analisar os equipamentos e verificar se está tudo certo com os firewalls da loja.</t>
+        </is>
+      </c>
+      <c r="O11" s="26" t="n"/>
+    </row>
+    <row r="12" ht="75" customHeight="1">
+      <c r="A12" s="26" t="inlineStr">
+        <is>
+          <t>Loja 161</t>
+        </is>
+      </c>
+      <c r="B12" s="26" t="inlineStr">
+        <is>
+          <t>R05 - Diely</t>
+        </is>
+      </c>
+      <c r="C12" s="31" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="D12" s="31" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E12" s="26" t="inlineStr">
+        <is>
+          <t>FALTA DE ENERGIA</t>
+        </is>
+      </c>
+      <c r="F12" s="26" t="inlineStr">
+        <is>
+          <t>ENERGIA</t>
+        </is>
+      </c>
+      <c r="G12" s="26" t="inlineStr">
+        <is>
+          <t>INOPERANTE</t>
+        </is>
+      </c>
+      <c r="H12" s="26" t="inlineStr">
+        <is>
+          <t>OI DEDICADO</t>
+        </is>
+      </c>
+      <c r="I12" s="28" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J12" s="32" t="inlineStr">
+        <is>
+          <t>25/06/2025 07:00</t>
+        </is>
+      </c>
+      <c r="K12" s="32" t="inlineStr">
+        <is>
+          <t>25/06/2025 09:00</t>
+        </is>
+      </c>
+      <c r="L12" s="30" t="inlineStr">
+        <is>
+          <t>02:00</t>
+        </is>
+      </c>
+      <c r="M12" s="27" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="N12" s="26" t="inlineStr">
+        <is>
+          <t>Identificado problema referente ao quadro de energia, um curto em um fusível do painel de energia, Nobreak sustentou a loja até o fim da autonomia, Gerente acompanhou o time de manutenção na correção do quadro de energia, energia normalizada, VMs e APIs religadas, Loja operando novamente.</t>
+        </is>
+      </c>
+      <c r="O12" s="26" t="n"/>
+    </row>
+    <row r="13" ht="75" customHeight="1">
+      <c r="A13" s="26" t="inlineStr">
+        <is>
+          <t>Loja 150</t>
+        </is>
+      </c>
+      <c r="B13" s="26" t="inlineStr">
+        <is>
+          <t>R09 - Edimar</t>
+        </is>
+      </c>
+      <c r="C13" s="31" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="D13" s="31" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="E13" s="26" t="inlineStr">
+        <is>
+          <t>LINK INOPERANTE</t>
+        </is>
+      </c>
+      <c r="F13" s="26" t="inlineStr">
+        <is>
+          <t>LINK</t>
+        </is>
+      </c>
+      <c r="G13" s="26" t="inlineStr">
+        <is>
+          <t>INOPERANTE</t>
+        </is>
+      </c>
+      <c r="H13" s="26" t="inlineStr">
+        <is>
+          <t>NENHUM</t>
+        </is>
+      </c>
+      <c r="I13" s="28" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J13" s="32" t="inlineStr">
+        <is>
+          <t>25/06/2025 06:00</t>
+        </is>
+      </c>
+      <c r="K13" s="32" t="inlineStr">
+        <is>
+          <t>25/06/2025 08:28</t>
+        </is>
+      </c>
+      <c r="L13" s="30" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="M13" s="27" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="N13" s="26" t="inlineStr">
+        <is>
+          <t>Foi identificado que a loja ficou Offline devido a ambos links ficarem Down, após analise dos times de rede, foi realizado reset nos aparelhos da operadora e no Switch, Link Principal voltou a responder e conexão da loja normalizada, Link Secundário segue Down em tratativa com a Operadora. Validado pelo time de Suporte em WR.</t>
+        </is>
+      </c>
+      <c r="O13" s="26" t="n"/>
+    </row>
+    <row r="14" ht="75" customHeight="1">
+      <c r="A14" s="26" t="inlineStr">
+        <is>
+          <t>Loja 58</t>
+        </is>
+      </c>
+      <c r="B14" s="26" t="inlineStr">
+        <is>
+          <t>R02 - Jonatas</t>
+        </is>
+      </c>
+      <c r="C14" s="31" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="D14" s="31" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="E14" s="26" t="inlineStr">
+        <is>
+          <t>FALTA DE ENERGIA</t>
+        </is>
+      </c>
+      <c r="F14" s="26" t="inlineStr">
+        <is>
+          <t>ENERGIA</t>
+        </is>
+      </c>
+      <c r="G14" s="26" t="inlineStr">
+        <is>
+          <t>INOPERANTE</t>
+        </is>
+      </c>
+      <c r="H14" s="26" t="inlineStr">
+        <is>
+          <t>OI DEDICADO</t>
+        </is>
+      </c>
+      <c r="I14" s="28" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J14" s="32" t="inlineStr">
+        <is>
+          <t>25/06/2025 06:00</t>
+        </is>
+      </c>
+      <c r="K14" s="32" t="inlineStr">
+        <is>
+          <t>25/06/2025 08:55</t>
+        </is>
+      </c>
+      <c r="L14" s="30" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="M14" s="27" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="N14" s="26" t="inlineStr">
+        <is>
+          <t>Foi identificado que as VMs da Loja estavam down devido a uma queda de energia na noite anterior, energia normalizada, equipamentos, VMs e APIs ligados novamente, Loja normalizada validado com Colaborador Luiz.</t>
+        </is>
+      </c>
+      <c r="O14" s="26" t="n"/>
+    </row>
+    <row r="15" ht="75" customHeight="1">
+      <c r="A15" s="26" t="inlineStr">
+        <is>
+          <t>Loja 161</t>
+        </is>
+      </c>
+      <c r="B15" s="26" t="inlineStr">
+        <is>
+          <t>R05 - Diely</t>
+        </is>
+      </c>
+      <c r="C15" s="31" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="D15" s="31" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E15" s="26" t="inlineStr">
+        <is>
+          <t>FALTA DE ENERGIA</t>
+        </is>
+      </c>
+      <c r="F15" s="26" t="inlineStr">
+        <is>
+          <t>ENERGIA</t>
+        </is>
+      </c>
+      <c r="G15" s="26" t="inlineStr">
+        <is>
+          <t>INOPERANTE</t>
+        </is>
+      </c>
+      <c r="H15" s="26" t="inlineStr">
+        <is>
+          <t>NENHUM</t>
+        </is>
+      </c>
+      <c r="I15" s="28" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J15" s="32" t="inlineStr">
+        <is>
+          <t>24/06/2025 17:40</t>
+        </is>
+      </c>
+      <c r="K15" s="32" t="inlineStr">
+        <is>
+          <t>24/06/2025 19:00</t>
+        </is>
+      </c>
+      <c r="L15" s="30" t="inlineStr">
+        <is>
+          <t>01:20</t>
+        </is>
+      </c>
+      <c r="M15" s="27" t="inlineStr">
+        <is>
+          <t>10:40</t>
+        </is>
+      </c>
+      <c r="N15" s="26" t="inlineStr">
+        <is>
+          <t>Houve um curto de fusível do painel de energia a loja encerrou o expediente, mas a gerente acompanhei o time da manutenção, pois o nobreak descarregou e a normalização da energia continua sem prazo para normalização. Aguardando normalização da energia e análise do nobreak para ver se seria necessário desligar os equipamentos ou não.</t>
+        </is>
+      </c>
+      <c r="O15" s="26" t="n"/>
+    </row>
+    <row r="16" ht="75" customHeight="1">
+      <c r="A16" s="26" t="inlineStr">
+        <is>
+          <t>Loja 47</t>
+        </is>
+      </c>
+      <c r="B16" s="26" t="inlineStr">
+        <is>
+          <t>R08 - Edimar</t>
+        </is>
+      </c>
+      <c r="C16" s="26" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D16" s="26" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E16" s="26" t="inlineStr">
+        <is>
+          <t>SERVIDOR DESLIGADO</t>
+        </is>
+      </c>
+      <c r="F16" s="26" t="inlineStr">
+        <is>
+          <t>SERVIÇO</t>
+        </is>
+      </c>
+      <c r="G16" s="26" t="inlineStr">
+        <is>
+          <t>INOPERANTE</t>
+        </is>
+      </c>
+      <c r="H16" s="26" t="inlineStr">
+        <is>
+          <t>NENHUM</t>
+        </is>
+      </c>
+      <c r="I16" s="26" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J16" s="26" t="inlineStr">
+        <is>
+          <t>24/06/2025 17:36</t>
+        </is>
+      </c>
+      <c r="K16" s="26" t="inlineStr">
+        <is>
+          <t>24/06/2025 19:00</t>
+        </is>
+      </c>
+      <c r="L16" s="26" t="inlineStr">
+        <is>
+          <t>01:24</t>
+        </is>
+      </c>
+      <c r="M16" s="26" t="inlineStr">
+        <is>
+          <t>09:36</t>
+        </is>
+      </c>
+      <c r="N16" s="26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loja desligou os equipamentos do rack de forma preventiva devido a chuva forte que alagou a sala da TI. Ficou no aguardo um retorno da loja para tratativa.  </t>
+        </is>
+      </c>
+      <c r="O16" s="26" t="n"/>
+    </row>
+    <row r="17" ht="75" customHeight="1">
+      <c r="A17" s="26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loja 119 </t>
+        </is>
+      </c>
+      <c r="B17" s="26" t="inlineStr">
+        <is>
+          <t>R07 - Willian Beycon</t>
+        </is>
+      </c>
+      <c r="C17" s="26" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="D17" s="26" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E17" s="26" t="inlineStr">
+        <is>
+          <t>LINK INOPERANTE</t>
+        </is>
+      </c>
+      <c r="F17" s="26" t="inlineStr">
+        <is>
+          <t>LINK</t>
+        </is>
+      </c>
+      <c r="G17" s="26" t="inlineStr">
+        <is>
+          <t>PARCIAL</t>
+        </is>
+      </c>
+      <c r="H17" s="26" t="inlineStr">
+        <is>
+          <t>NENHUM</t>
+        </is>
+      </c>
+      <c r="I17" s="26" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J17" s="26" t="inlineStr">
+        <is>
+          <t>24/06/2025 17:35</t>
+        </is>
+      </c>
+      <c r="K17" s="26" t="inlineStr">
+        <is>
+          <t>24/06/2025 17:50</t>
+        </is>
+      </c>
+      <c r="L17" s="26" t="inlineStr">
+        <is>
+          <t>00:15</t>
+        </is>
+      </c>
+      <c r="M17" s="26" t="inlineStr">
+        <is>
+          <t>11:45</t>
+        </is>
+      </c>
+      <c r="N17" s="26" t="inlineStr">
+        <is>
+          <t>Loja se encontrava sem sistema Var para operações devido a ambos os links terem ficado down. Confirmado com o suporte que a loja estava vendendo offline até a normalização do link. Aberto chamado com a operadora para verificação, o link secundário ficou up e estável então foi solicitado ao suporte acompanhar a loja em um teste de venda e validar a VENDA ONLINE, que foi validado pela Larissa. Sem retorno da operadora quanto a solução. Protocolo Link principal: 91855659895 | Protocolo Link Secundário: 91855660874.</t>
+        </is>
+      </c>
+      <c r="O17" s="26" t="n"/>
+    </row>
+    <row r="18" ht="75" customHeight="1">
+      <c r="A18" s="26" t="inlineStr">
+        <is>
+          <t>Loja 20</t>
+        </is>
+      </c>
+      <c r="B18" s="26" t="inlineStr">
+        <is>
+          <t>R02 - Jonatas</t>
+        </is>
+      </c>
+      <c r="C18" s="26" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D18" s="26" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="E18" s="26" t="inlineStr">
+        <is>
+          <t>SERVIDOR DESLIGADO</t>
+        </is>
+      </c>
+      <c r="F18" s="26" t="inlineStr">
+        <is>
+          <t>SERVIÇO</t>
+        </is>
+      </c>
+      <c r="G18" s="26" t="inlineStr">
+        <is>
+          <t>INOPERANTE</t>
+        </is>
+      </c>
+      <c r="H18" s="26" t="inlineStr">
+        <is>
+          <t>NENHUM</t>
+        </is>
+      </c>
+      <c r="I18" s="26" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J18" s="26" t="inlineStr">
+        <is>
+          <t>24/06/2025 06:00</t>
+        </is>
+      </c>
+      <c r="K18" s="26" t="inlineStr">
+        <is>
+          <t>24/06/2025 18:00</t>
+        </is>
+      </c>
+      <c r="L18" s="26" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="M18" s="26" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="N18" s="26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loja passando por manutenção no ESXI, então os equipamentos foram desligados. Aguardando finalizar a manutenção para religar os equipamentos e realizar teste de venda. </t>
+        </is>
+      </c>
+      <c r="O18" s="26" t="n"/>
+    </row>
+    <row r="19" ht="75" customHeight="1">
+      <c r="A19" s="26" t="inlineStr">
+        <is>
+          <t>Loja 47</t>
+        </is>
+      </c>
+      <c r="B19" s="26" t="inlineStr">
+        <is>
+          <t>R08 - Edimar</t>
+        </is>
+      </c>
+      <c r="C19" s="26" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D19" s="26" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E19" s="26" t="inlineStr">
+        <is>
+          <t>SERVIDOR DESLIGADO</t>
+        </is>
+      </c>
+      <c r="F19" s="26" t="inlineStr">
+        <is>
+          <t>SERVIÇO</t>
+        </is>
+      </c>
+      <c r="G19" s="26" t="inlineStr">
+        <is>
+          <t>INOPERANTE</t>
+        </is>
+      </c>
+      <c r="H19" s="26" t="inlineStr">
+        <is>
+          <t>NENHUM</t>
+        </is>
+      </c>
+      <c r="I19" s="26" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J19" s="26" t="inlineStr">
+        <is>
+          <t>23/06/2025 16:50</t>
+        </is>
+      </c>
+      <c r="K19" s="26" t="inlineStr">
+        <is>
+          <t>23/06/2025 17:56</t>
+        </is>
+      </c>
+      <c r="L19" s="26" t="inlineStr">
+        <is>
+          <t>01:06</t>
+        </is>
+      </c>
+      <c r="M19" s="26" t="inlineStr">
+        <is>
+          <t>09:54</t>
+        </is>
+      </c>
+      <c r="N19" s="26" t="inlineStr">
+        <is>
+          <t>Equipamentos da loja ficaram down, a loja desligou o nobreak pois estava apitando enquanto limpavam a sala da TI que alagou devido a chuva. Assim que limparam a sala da ti, o time de redes religou as VMs. Solicitado ao suporte acompanhar a loja em um teste de venda que foi validada pela Glória. Ao encerrar o expediente foi desligado os equipamentos de forma preventiva pela equipe de redes.</t>
+        </is>
+      </c>
+      <c r="O19" s="26" t="n"/>
+    </row>
+    <row r="20" ht="75" customHeight="1">
+      <c r="A20" s="26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loja 119 </t>
+        </is>
+      </c>
+      <c r="B20" s="26" t="inlineStr">
+        <is>
+          <t>R07 - Willian Beycon</t>
+        </is>
+      </c>
+      <c r="C20" s="26" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="D20" s="26" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E20" s="26" t="inlineStr">
+        <is>
+          <t>FALTA DE ENERGIA</t>
+        </is>
+      </c>
+      <c r="F20" s="26" t="inlineStr">
+        <is>
+          <t>NOBREAK</t>
+        </is>
+      </c>
+      <c r="G20" s="26" t="inlineStr">
+        <is>
+          <t>PARCIAL</t>
+        </is>
+      </c>
+      <c r="H20" s="26" t="inlineStr">
+        <is>
+          <t>OI DEDICADO</t>
+        </is>
+      </c>
+      <c r="I20" s="26" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J20" s="26" t="inlineStr">
+        <is>
+          <t>23/06/2025 11:16</t>
+        </is>
+      </c>
+      <c r="K20" s="26" t="inlineStr">
+        <is>
+          <t>23/06/2025 14:09</t>
+        </is>
+      </c>
+      <c r="L20" s="26" t="inlineStr">
+        <is>
+          <t>02:53</t>
+        </is>
+      </c>
+      <c r="M20" s="26" t="inlineStr">
+        <is>
+          <t>09:07</t>
+        </is>
+      </c>
+      <c r="N20" s="26" t="inlineStr">
+        <is>
+          <t>Houve queda de energia na região, sem retorno da concessionária quanto a causa. Após a energia ter sido normalizada as VMs e APIs serem religadas os equipamentos ficaram novamente. Solicitado ao suporte acompanhar a loja em um teste de venda que foi validado pela Eliane.</t>
+        </is>
+      </c>
+      <c r="O20" s="26" t="n"/>
+    </row>
+    <row r="21" ht="75" customHeight="1">
+      <c r="A21" s="26" t="inlineStr">
+        <is>
           <t>Loja 10</t>
         </is>
       </c>
-      <c r="B6" s="26" t="inlineStr">
+      <c r="B21" s="26" t="inlineStr">
         <is>
           <t>R04 - Marilete</t>
         </is>
       </c>
-      <c r="C6" s="26" t="inlineStr">
+      <c r="C21" s="26" t="inlineStr">
         <is>
           <t>10:00</t>
         </is>
       </c>
-      <c r="D6" s="26" t="inlineStr">
+      <c r="D21" s="26" t="inlineStr">
         <is>
           <t>22:00</t>
         </is>
       </c>
-      <c r="E6" s="26" t="inlineStr">
+      <c r="E21" s="26" t="inlineStr">
         <is>
           <t>SERVIDOR DESLIGADO</t>
         </is>
       </c>
-      <c r="F6" s="26" t="inlineStr">
+      <c r="F21" s="26" t="inlineStr">
         <is>
           <t>SERVIDOR</t>
         </is>
       </c>
-      <c r="G6" s="26" t="inlineStr">
+      <c r="G21" s="26" t="inlineStr">
         <is>
           <t>INOPERANTE</t>
         </is>
       </c>
-      <c r="H6" s="26" t="inlineStr">
+      <c r="H21" s="26" t="inlineStr">
         <is>
           <t>NENHUM</t>
         </is>
       </c>
-      <c r="I6" s="26" t="inlineStr">
-        <is>
-          <t>26/06/2025</t>
-        </is>
-      </c>
-      <c r="J6" s="26" t="inlineStr">
+      <c r="I21" s="26" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J21" s="26" t="inlineStr">
         <is>
           <t>23/06/2025 07:00</t>
         </is>
       </c>
-      <c r="K6" s="26" t="inlineStr">
+      <c r="K21" s="26" t="inlineStr">
         <is>
           <t>23/06/2025 10:15</t>
         </is>
       </c>
-      <c r="L6" s="26" t="inlineStr">
+      <c r="L21" s="26" t="inlineStr">
         <is>
           <t>00:15</t>
         </is>
       </c>
-      <c r="M6" s="26" t="inlineStr">
+      <c r="M21" s="26" t="inlineStr">
         <is>
           <t>11:45</t>
         </is>
       </c>
-      <c r="N6" s="26" t="inlineStr">
+      <c r="N21" s="26" t="inlineStr">
         <is>
           <t>Os equipamentos não estavam respondendo o time de redes ficou aguardando retorno da loja. VMs e APIs foram religadas e ficaram UPs, os equipamentos voltaram a responder e foi solicitado ao suporte acompanhar a loja em um teste de venda. Validado pela Yasmin.</t>
         </is>
       </c>
+      <c r="O21" s="26" t="n"/>
     </row>
-    <row r="7" ht="56.25" customHeight="1">
-      <c r="A7" s="10" t="n"/>
-      <c r="B7" s="10" t="n"/>
-      <c r="C7" s="20" t="n"/>
-      <c r="D7" s="20" t="n"/>
-      <c r="E7" s="10" t="n"/>
-      <c r="F7" s="10" t="n"/>
-      <c r="G7" s="10" t="n"/>
-      <c r="H7" s="10" t="n"/>
-      <c r="I7" s="27" t="n"/>
-      <c r="J7" s="21" t="n"/>
-      <c r="K7" s="22" t="n"/>
-      <c r="L7" s="12" t="n"/>
-      <c r="M7" s="13" t="n"/>
-      <c r="N7" s="18" t="n"/>
-      <c r="O7" s="14" t="n"/>
+    <row r="22" ht="75" customHeight="1">
+      <c r="A22" s="26" t="inlineStr">
+        <is>
+          <t>LOJA 210</t>
+        </is>
+      </c>
+      <c r="B22" s="26" t="inlineStr">
+        <is>
+          <t>R06 - Drielly</t>
+        </is>
+      </c>
+      <c r="C22" s="26" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D22" s="26" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="E22" s="26" t="inlineStr">
+        <is>
+          <t>FALTA DE ENERGIA</t>
+        </is>
+      </c>
+      <c r="F22" s="26" t="inlineStr">
+        <is>
+          <t>SERVIÇO</t>
+        </is>
+      </c>
+      <c r="G22" s="26" t="inlineStr">
+        <is>
+          <t>INOPERANTE</t>
+        </is>
+      </c>
+      <c r="H22" s="26" t="inlineStr">
+        <is>
+          <t>NENHUM</t>
+        </is>
+      </c>
+      <c r="I22" s="26" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J22" s="26" t="inlineStr">
+        <is>
+          <t>23/06/2025 07:00</t>
+        </is>
+      </c>
+      <c r="K22" s="26" t="inlineStr">
+        <is>
+          <t>23/06/2025 08:03</t>
+        </is>
+      </c>
+      <c r="L22" s="26" t="inlineStr">
+        <is>
+          <t>00:03</t>
+        </is>
+      </c>
+      <c r="M22" s="26" t="inlineStr">
+        <is>
+          <t>09:57</t>
+        </is>
+      </c>
+      <c r="N22" s="26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loja teve o disjuntor desligado no fechamento da loja, pois uma cortina de ar pegou fogo e o gerente desligou o disjuntor geral para controlar o fogo. Foi religado o disjuntor e os equipamentos ficaram Ups novamente. Solicitado ao suporte acompanhar a loja em um teste de venda que foi validado pelo Rodolfo.  </t>
+        </is>
+      </c>
+      <c r="O22" s="26" t="n"/>
     </row>
-    <row r="8" ht="56.25" customHeight="1"/>
-    <row r="9" ht="56.25" customHeight="1"/>
-    <row r="10" ht="56.25" customHeight="1"/>
-    <row r="11" ht="56.25" customHeight="1"/>
-    <row r="12" ht="56.25" customHeight="1"/>
-    <row r="13" ht="56.25" customHeight="1"/>
-    <row r="14" ht="56.25" customHeight="1"/>
-    <row r="15" ht="56.25" customHeight="1"/>
+    <row r="23" ht="75" customHeight="1">
+      <c r="A23" s="26" t="inlineStr">
+        <is>
+          <t>Loja 123</t>
+        </is>
+      </c>
+      <c r="B23" s="26" t="inlineStr">
+        <is>
+          <t>R08 - Edimar</t>
+        </is>
+      </c>
+      <c r="C23" s="26" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="D23" s="26" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E23" s="26" t="inlineStr">
+        <is>
+          <t>FALTA DE ENERGIA</t>
+        </is>
+      </c>
+      <c r="F23" s="26" t="inlineStr">
+        <is>
+          <t>NOBREAK</t>
+        </is>
+      </c>
+      <c r="G23" s="26" t="inlineStr">
+        <is>
+          <t>INOPERANTE</t>
+        </is>
+      </c>
+      <c r="H23" s="26" t="inlineStr">
+        <is>
+          <t>NENHUM</t>
+        </is>
+      </c>
+      <c r="I23" s="26" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="J23" s="26" t="inlineStr">
+        <is>
+          <t>23/06/2025 07:00</t>
+        </is>
+      </c>
+      <c r="K23" s="26" t="inlineStr">
+        <is>
+          <t>23/06/2025 07:50</t>
+        </is>
+      </c>
+      <c r="L23" s="26" t="inlineStr">
+        <is>
+          <t>00:50</t>
+        </is>
+      </c>
+      <c r="M23" s="26" t="inlineStr">
+        <is>
+          <t>11:10</t>
+        </is>
+      </c>
+      <c r="N23" s="26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Os equipamentos da loja não respondiam mesmo com a chave virada para o nobreak. Nobreak da loja apresentou falha, foi solicitado ao ECA que ficou de enviar técnico para verificar o nobreak. Após normalização a chave foi virada novamente para rede e os equipamentos ficaram Ups novamente. </t>
+        </is>
+      </c>
+      <c r="O23" s="26" t="n"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
add lógica para automatizacao do calculo de impacto e indisponibilidade
</commit_message>
<xml_diff>
--- a/Incidentes_Formatados_Final.xlsx
+++ b/Incidentes_Formatados_Final.xlsx
@@ -783,7 +783,7 @@
       </c>
       <c r="M2" s="27" t="inlineStr">
         <is>
-          <t>09:28</t>
+          <t>13:28</t>
         </is>
       </c>
       <c r="N2" s="26" t="inlineStr">
@@ -1368,7 +1368,7 @@
       </c>
       <c r="M10" s="27" t="inlineStr">
         <is>
-          <t>08:32</t>
+          <t>14:32</t>
         </is>
       </c>
       <c r="N10" s="26" t="inlineStr">
@@ -1587,7 +1587,7 @@
       </c>
       <c r="M13" s="27" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="N13" s="26" t="inlineStr">
@@ -1660,7 +1660,7 @@
       </c>
       <c r="M14" s="27" t="inlineStr">
         <is>
-          <t>00:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="N14" s="26" t="inlineStr">

</xml_diff>